<commit_message>
chapter 4 2D case
</commit_message>
<xml_diff>
--- a/xjh/TEST/turb_flat_plate/postprocess.xlsx
+++ b/xjh/TEST/turb_flat_plate/postprocess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xjh/thesis/xjh/TEST/turb_flat_plate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B409C5CB-C7BF-E945-B36C-0562B02912AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6359514-5724-BD43-90EA-BAD1DB5F0C06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="8" xr2:uid="{E813E3D2-8B92-5C49-8DD6-185F646B6F3F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="6" xr2:uid="{E813E3D2-8B92-5C49-8DD6-185F646B6F3F}"/>
   </bookViews>
   <sheets>
     <sheet name="coarse_CPU" sheetId="1" r:id="rId1"/>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BEE77C-FC9B-2A4B-B70C-ACB86D236C97}">
   <dimension ref="A1:BP256"/>
   <sheetViews>
-    <sheetView topLeftCell="E26" zoomScale="83" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="P54" sqref="P54"/>
+    <sheetView topLeftCell="A26" zoomScale="83" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="K54" sqref="B54:K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8857,8 +8857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E60AECBB-FA79-814B-BF8F-04A58F7DEA5D}">
   <dimension ref="A1:AA137"/>
   <sheetViews>
-    <sheetView topLeftCell="J32" zoomScale="88" workbookViewId="0">
-      <selection activeCell="O56" sqref="O56"/>
+    <sheetView topLeftCell="A25" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55:I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11602,8 +11602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01678F02-6852-1843-B1D7-578F6A92EC72}">
   <dimension ref="A1:T155"/>
   <sheetViews>
-    <sheetView topLeftCell="I32" zoomScale="113" workbookViewId="0">
-      <selection activeCell="M55" sqref="M55"/>
+    <sheetView topLeftCell="A36" zoomScale="109" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55:I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14319,8 +14319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{997AAC41-7DA1-1B44-A5DD-D52E7253628E}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView topLeftCell="I19" workbookViewId="0">
-      <selection activeCell="P54" sqref="P54"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54:K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -16427,8 +16427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC127979-67F1-E34D-A955-D458C318AA63}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView topLeftCell="G21" workbookViewId="0">
-      <selection activeCell="M55" sqref="M55"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="I55" sqref="C55:I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18789,8 +18789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5B5681-45AC-0346-9654-EB9601C24614}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView topLeftCell="G20" workbookViewId="0">
-      <selection activeCell="M55" sqref="M55"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55:I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -21154,8 +21154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53BD7A38-7217-2548-973C-208A00C6B180}">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P53" sqref="P53"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -23180,7 +23180,10 @@
       </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
+      <c r="K53" s="3">
+        <f>AVERAGE(K2:K52)</f>
+        <v>0.84779874000000011</v>
+      </c>
       <c r="L53" s="3"/>
       <c r="M53" s="3">
         <f>AVERAGE(M2:M52)</f>
@@ -23212,8 +23215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAEEC0B4-D074-4C48-ABA5-AA0B4D84D4DC}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView topLeftCell="H27" workbookViewId="0">
-      <selection activeCell="M55" sqref="M55"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55:I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -25574,8 +25577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262195B1-C42F-1044-B686-6150185ED2A3}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C55" sqref="C55:I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>